<commit_message>
Update binary.py in function 2
</commit_message>
<xml_diff>
--- a/out/results_2024-03-04.xlsx
+++ b/out/results_2024-03-04.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2994,6 +2994,378 @@
         <v>34227</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>1</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>5-4-4</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>4161</v>
+      </c>
+      <c r="G84" t="n">
+        <v>34227</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>1</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F85" t="n">
+        <v>168</v>
+      </c>
+      <c r="G85" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>1</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F86" t="n">
+        <v>168</v>
+      </c>
+      <c r="G86" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>1</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>168</v>
+      </c>
+      <c r="G87" t="n">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>1</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>169</v>
+      </c>
+      <c r="G88" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>1</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>169</v>
+      </c>
+      <c r="G89" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>1</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F90" t="n">
+        <v>169</v>
+      </c>
+      <c r="G90" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>1</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F91" t="n">
+        <v>169</v>
+      </c>
+      <c r="G91" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>1</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>3-2-2</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F92" t="n">
+        <v>169</v>
+      </c>
+      <c r="G92" t="n">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>1</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>6-5-5</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>timeout</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>timeout</t>
+        </is>
+      </c>
+      <c r="F93" t="n">
+        <v>12002</v>
+      </c>
+      <c r="G93" t="n">
+        <v>160072</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>1</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>6-5-5</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>binomial</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>33.672</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F94" t="n">
+        <v>4500</v>
+      </c>
+      <c r="G94" t="n">
+        <v>167615</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>1</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>6-5-5</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>9.625</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="F95" t="n">
+        <v>12002</v>
+      </c>
+      <c r="G95" t="n">
+        <v>157640</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>